<commit_message>
new tibble update adjustments
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/j.schwarz/Documents/06_gh_page/data-science/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD102AA-800E-F54B-904E-6D873CE2623D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95D317CB-57F7-334B-958C-BF09E2D88436}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33920" yWindow="3760" windowWidth="25520" windowHeight="15540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-33620" yWindow="8060" windowWidth="25520" windowHeight="15540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>Date</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>Lab</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -416,7 +419,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -442,7 +445,12 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="B2" s="2"/>
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="C2" s="1" t="s">
         <v>10</v>
       </c>

</xml_diff>